<commit_message>
Major modification in datasets
The 3 and 10 bus cdf files were not of the correct dimensions and this led to issues in creating the final output. It has been corrected.

The calcMain files also have new lines to account for these datasets that are not in PU format. But it is only for testing purposes and will not be used for the 33bus system
</commit_message>
<xml_diff>
--- a/Documentations/Datasets/10busCDF.xlsx
+++ b/Documentations/Datasets/10busCDF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\Ladder-Iterative-Loadflow\Documentations\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C722AC4-C37D-4A86-A7D7-71C7C077BAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF0ED17-D61B-44E5-951E-96B89F58853B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{AE3323F2-0094-4B0C-9BAF-50E26493BB40}"/>
+    <workbookView xWindow="-510" yWindow="3450" windowWidth="21600" windowHeight="11475" xr2:uid="{AE3323F2-0094-4B0C-9BAF-50E26493BB40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>END OF DATA</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>11/13/21 RYERSON UNIVERSITY  100.0  2021 W IEEE 33 Bus Test Case</t>
+  </si>
+  <si>
+    <t>Bus 10</t>
   </si>
 </sst>
 </file>
@@ -492,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02368925-FB68-47DE-A660-EAA97F9F58F2}">
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -599,10 +602,10 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="H4" s="11">
-        <v>0.1</v>
+        <v>1500</v>
       </c>
       <c r="I4" s="11">
-        <v>0.06</v>
+        <v>750</v>
       </c>
       <c r="J4" s="2">
         <v>0</v>
@@ -655,10 +658,10 @@
         <v>9.9599999999999994E-2</v>
       </c>
       <c r="H5" s="11">
-        <v>0.09</v>
+        <v>900</v>
       </c>
       <c r="I5" s="11">
-        <v>0.04</v>
+        <v>500</v>
       </c>
       <c r="J5" s="2">
         <v>0</v>
@@ -711,10 +714,10 @@
         <v>0.16769999999999999</v>
       </c>
       <c r="H6" s="11">
-        <v>0.12</v>
+        <v>800</v>
       </c>
       <c r="I6" s="11">
-        <v>0.08</v>
+        <v>450</v>
       </c>
       <c r="J6" s="2">
         <v>0</v>
@@ -767,10 +770,10 @@
         <v>0.2369</v>
       </c>
       <c r="H7" s="11">
-        <v>0.06</v>
+        <v>700</v>
       </c>
       <c r="I7" s="11">
-        <v>0.03</v>
+        <v>400</v>
       </c>
       <c r="J7" s="2">
         <v>0</v>
@@ -823,10 +826,10 @@
         <v>0.14549999999999999</v>
       </c>
       <c r="H8" s="11">
-        <v>0.06</v>
+        <v>600</v>
       </c>
       <c r="I8" s="11">
-        <v>0.02</v>
+        <v>350</v>
       </c>
       <c r="J8" s="2">
         <v>0</v>
@@ -879,10 +882,10 @@
         <v>-8.5099999999999995E-2</v>
       </c>
       <c r="H9" s="11">
-        <v>0.2</v>
+        <v>500</v>
       </c>
       <c r="I9" s="11">
-        <v>0.1</v>
+        <v>300</v>
       </c>
       <c r="J9" s="2">
         <v>0</v>
@@ -935,10 +938,10 @@
         <v>-4.9000000000000002E-2</v>
       </c>
       <c r="H10" s="11">
-        <v>0.2</v>
+        <v>400</v>
       </c>
       <c r="I10" s="11">
-        <v>0.1</v>
+        <v>250</v>
       </c>
       <c r="J10" s="2">
         <v>0</v>
@@ -991,10 +994,10 @@
         <v>-0.1222</v>
       </c>
       <c r="H11" s="11">
-        <v>0.06</v>
+        <v>300</v>
       </c>
       <c r="I11" s="11">
-        <v>0.02</v>
+        <v>200</v>
       </c>
       <c r="J11" s="2">
         <v>0</v>
@@ -1025,93 +1028,84 @@
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0.9345</v>
+      </c>
+      <c r="G12" s="10">
+        <v>-0.1222</v>
+      </c>
+      <c r="H12" s="11">
+        <v>200</v>
+      </c>
+      <c r="I12" s="11">
+        <v>100</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>12.66</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="3">
         <v>-999</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:21">
+      <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="U13" s="2"/>
-    </row>
-    <row r="14" spans="1:21">
-      <c r="A14" s="5">
-        <v>1</v>
-      </c>
-      <c r="B14" s="5">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="7">
-        <v>5.7500000000000002E-2</v>
-      </c>
-      <c r="H14" s="7">
-        <v>2.93E-2</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
-        <v>0</v>
-      </c>
-      <c r="L14" s="2">
-        <v>0</v>
-      </c>
-      <c r="M14" s="2">
-        <v>0</v>
-      </c>
-      <c r="N14" s="2">
-        <v>0</v>
-      </c>
-      <c r="O14" s="2">
-        <v>0</v>
-      </c>
-      <c r="P14" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>0</v>
-      </c>
-      <c r="R14" s="2">
-        <v>0</v>
-      </c>
-      <c r="S14" s="2">
-        <v>0</v>
-      </c>
-      <c r="T14" s="2">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="U14" s="2">
-        <v>4.5999999999999996</v>
-      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="U14" s="2"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="5">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5">
         <v>2</v>
       </c>
-      <c r="B15" s="5">
-        <v>3</v>
-      </c>
       <c r="C15" s="2">
         <v>1</v>
       </c>
@@ -1125,10 +1119,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="7">
-        <v>0.30759999999999998</v>
+        <v>0.17050000000000001</v>
       </c>
       <c r="H15" s="7">
-        <v>0.15670000000000001</v>
+        <v>0.34089999999999998</v>
       </c>
       <c r="I15" s="2">
         <v>0</v>
@@ -1164,19 +1158,19 @@
         <v>0</v>
       </c>
       <c r="T15" s="2">
-        <v>4.0999999999999996</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="U15" s="2">
-        <v>4.0999999999999996</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="5">
+        <v>2</v>
+      </c>
+      <c r="B16" s="5">
         <v>3</v>
       </c>
-      <c r="B16" s="5">
-        <v>4</v>
-      </c>
       <c r="C16" s="2">
         <v>1</v>
       </c>
@@ -1190,10 +1184,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="7">
-        <v>0.22839999999999999</v>
+        <v>0.2273</v>
       </c>
       <c r="H16" s="7">
-        <v>0.1163</v>
+        <v>0.45450000000000002</v>
       </c>
       <c r="I16" s="2">
         <v>0</v>
@@ -1229,19 +1223,19 @@
         <v>0</v>
       </c>
       <c r="T16" s="2">
-        <v>2.9</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="U16" s="2">
-        <v>2.9</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="17" spans="1:21">
       <c r="A17" s="5">
+        <v>3</v>
+      </c>
+      <c r="B17" s="5">
         <v>4</v>
       </c>
-      <c r="B17" s="5">
-        <v>5</v>
-      </c>
       <c r="C17" s="2">
         <v>1</v>
       </c>
@@ -1255,10 +1249,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="7">
-        <v>0.23780000000000001</v>
+        <v>0.2273</v>
       </c>
       <c r="H17" s="7">
-        <v>0.1211</v>
+        <v>0.45450000000000002</v>
       </c>
       <c r="I17" s="2">
         <v>0</v>
@@ -1302,11 +1296,11 @@
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="5">
+        <v>4</v>
+      </c>
+      <c r="B18" s="5">
         <v>5</v>
       </c>
-      <c r="B18" s="5">
-        <v>6</v>
-      </c>
       <c r="C18" s="2">
         <v>1</v>
       </c>
@@ -1320,10 +1314,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="7">
-        <v>0.51100000000000001</v>
+        <v>0.2273</v>
       </c>
       <c r="H18" s="7">
-        <v>0.44109999999999999</v>
+        <v>0.45450000000000002</v>
       </c>
       <c r="I18" s="2">
         <v>0</v>
@@ -1367,11 +1361,11 @@
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="5">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5">
         <v>6</v>
       </c>
-      <c r="B19" s="5">
-        <v>7</v>
-      </c>
       <c r="C19" s="2">
         <v>1</v>
       </c>
@@ -1385,10 +1379,10 @@
         <v>0</v>
       </c>
       <c r="G19" s="7">
-        <v>0.1168</v>
+        <v>0.2273</v>
       </c>
       <c r="H19" s="7">
-        <v>0.3861</v>
+        <v>0.45450000000000002</v>
       </c>
       <c r="I19" s="2">
         <v>0</v>
@@ -1424,19 +1418,19 @@
         <v>0</v>
       </c>
       <c r="T19" s="2">
-        <v>1.5</v>
+        <v>2.9</v>
       </c>
       <c r="U19" s="2">
-        <v>1.5</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="20" spans="1:21">
       <c r="A20" s="5">
+        <v>6</v>
+      </c>
+      <c r="B20" s="5">
         <v>7</v>
       </c>
-      <c r="B20" s="5">
-        <v>8</v>
-      </c>
       <c r="C20" s="2">
         <v>1</v>
       </c>
@@ -1450,10 +1444,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="7">
-        <v>0.44390000000000002</v>
+        <v>0.2273</v>
       </c>
       <c r="H20" s="7">
-        <v>0.1467</v>
+        <v>0.45450000000000002</v>
       </c>
       <c r="I20" s="2">
         <v>0</v>
@@ -1489,19 +1483,19 @@
         <v>0</v>
       </c>
       <c r="T20" s="2">
-        <v>1.05</v>
+        <v>1.5</v>
       </c>
       <c r="U20" s="2">
-        <v>1.05</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="21" spans="1:21">
       <c r="A21" s="5">
+        <v>7</v>
+      </c>
+      <c r="B21" s="5">
         <v>8</v>
       </c>
-      <c r="B21" s="5">
-        <v>9</v>
-      </c>
       <c r="C21" s="2">
         <v>1</v>
       </c>
@@ -1515,10 +1509,10 @@
         <v>0</v>
       </c>
       <c r="G21" s="7">
-        <v>0.64259999999999995</v>
+        <v>0.2273</v>
       </c>
       <c r="H21" s="7">
-        <v>0.4617</v>
+        <v>0.45450000000000002</v>
       </c>
       <c r="I21" s="2">
         <v>0</v>
@@ -1562,11 +1556,11 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="5">
+        <v>8</v>
+      </c>
+      <c r="B22" s="5">
         <v>9</v>
       </c>
-      <c r="B22" s="5">
-        <v>10</v>
-      </c>
       <c r="C22" s="2">
         <v>1</v>
       </c>
@@ -1580,10 +1574,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="7">
-        <v>0.65139999999999998</v>
+        <v>0.2273</v>
       </c>
       <c r="H22" s="7">
-        <v>0.4617</v>
+        <v>0.45450000000000002</v>
       </c>
       <c r="I22" s="2">
         <v>0</v>
@@ -1626,144 +1620,144 @@
       </c>
     </row>
     <row r="23" spans="1:21">
-      <c r="A23" s="3">
+      <c r="A23" s="5">
+        <v>9</v>
+      </c>
+      <c r="B23" s="5">
+        <v>10</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="7">
+        <v>0.2273</v>
+      </c>
+      <c r="H23" s="7">
+        <v>0.45450000000000002</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0</v>
+      </c>
+      <c r="O23" s="2">
+        <v>0</v>
+      </c>
+      <c r="P23" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>0</v>
+      </c>
+      <c r="R23" s="2">
+        <v>0</v>
+      </c>
+      <c r="S23" s="2">
+        <v>0</v>
+      </c>
+      <c r="T23" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="U23" s="2">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="A24" s="3">
         <v>-999</v>
-      </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="U23" s="2"/>
-    </row>
-    <row r="24" spans="1:21">
-      <c r="A24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="U24" s="2"/>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="2">
-        <v>1</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>19</v>
+      <c r="A25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="U25" s="2"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="3">
-        <v>-99</v>
+      <c r="A26" s="2">
+        <v>1</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="U26" s="2"/>
     </row>
     <row r="27" spans="1:21">
-      <c r="A27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>2</v>
+      <c r="A27" s="3">
+        <v>-99</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="U27" s="2"/>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" s="3">
-        <v>-9</v>
+      <c r="A28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="U28" s="2"/>
     </row>
     <row r="29" spans="1:21">
-      <c r="A29" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>20</v>
+      <c r="A29" s="3">
+        <v>-9</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="U29" s="2"/>
     </row>
     <row r="30" spans="1:21">
-      <c r="A30" s="5">
-        <v>8</v>
-      </c>
-      <c r="B30" s="5">
-        <v>21</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2">
-        <v>1</v>
-      </c>
-      <c r="E30" s="2">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0</v>
-      </c>
-      <c r="G30" s="7">
-        <v>0.50180000000000002</v>
-      </c>
-      <c r="H30" s="7">
-        <v>0.43709999999999999</v>
-      </c>
-      <c r="I30" s="2">
-        <v>0</v>
-      </c>
-      <c r="J30" s="2">
-        <v>0</v>
-      </c>
-      <c r="K30" s="2">
-        <v>0</v>
-      </c>
-      <c r="L30" s="2">
-        <v>0</v>
-      </c>
-      <c r="M30" s="2">
-        <v>0</v>
-      </c>
-      <c r="N30" s="2">
-        <v>0</v>
-      </c>
-      <c r="O30" s="2">
-        <v>0</v>
-      </c>
-      <c r="P30" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="2">
-        <v>0</v>
-      </c>
-      <c r="R30" s="2">
-        <v>0</v>
-      </c>
-      <c r="S30" s="2">
-        <v>0</v>
-      </c>
-      <c r="T30" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="U30" s="2">
-        <v>1.5</v>
-      </c>
+      <c r="A30" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="U30" s="2"/>
     </row>
     <row r="31" spans="1:21">
       <c r="A31" s="5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" s="5">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C31" s="2">
         <v>1</v>
@@ -1778,10 +1772,10 @@
         <v>0</v>
       </c>
       <c r="G31" s="7">
-        <v>0.31659999999999999</v>
+        <v>0.50180000000000002</v>
       </c>
       <c r="H31" s="7">
-        <v>0.1613</v>
+        <v>0.43709999999999999</v>
       </c>
       <c r="I31" s="2">
         <v>0</v>
@@ -1825,10 +1819,10 @@
     </row>
     <row r="32" spans="1:21">
       <c r="A32" s="5">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B32" s="5">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C32" s="2">
         <v>1</v>
@@ -1843,10 +1837,10 @@
         <v>0</v>
       </c>
       <c r="G32" s="7">
-        <v>0.60799999999999998</v>
+        <v>0.31659999999999999</v>
       </c>
       <c r="H32" s="7">
-        <v>0.6008</v>
+        <v>0.1613</v>
       </c>
       <c r="I32" s="2">
         <v>0</v>
@@ -1890,10 +1884,10 @@
     </row>
     <row r="33" spans="1:21">
       <c r="A33" s="5">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B33" s="5">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
@@ -1908,10 +1902,10 @@
         <v>0</v>
       </c>
       <c r="G33" s="7">
-        <v>0.19370000000000001</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="H33" s="7">
-        <v>0.2258</v>
+        <v>0.6008</v>
       </c>
       <c r="I33" s="2">
         <v>0</v>
@@ -1955,10 +1949,10 @@
     </row>
     <row r="34" spans="1:21">
       <c r="A34" s="5">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B34" s="5">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C34" s="2">
         <v>1</v>
@@ -1973,10 +1967,10 @@
         <v>0</v>
       </c>
       <c r="G34" s="7">
-        <v>0.21279999999999999</v>
+        <v>0.19370000000000001</v>
       </c>
       <c r="H34" s="7">
-        <v>0.33079999999999998</v>
+        <v>0.2258</v>
       </c>
       <c r="I34" s="2">
         <v>0</v>
@@ -2019,20 +2013,85 @@
       </c>
     </row>
     <row r="35" spans="1:21">
-      <c r="A35" s="3">
+      <c r="A35" s="5">
+        <v>25</v>
+      </c>
+      <c r="B35" s="5">
+        <v>29</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
+      <c r="G35" s="7">
+        <v>0.21279999999999999</v>
+      </c>
+      <c r="H35" s="7">
+        <v>0.33079999999999998</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2">
+        <v>0</v>
+      </c>
+      <c r="K35" s="2">
+        <v>0</v>
+      </c>
+      <c r="L35" s="2">
+        <v>0</v>
+      </c>
+      <c r="M35" s="2">
+        <v>0</v>
+      </c>
+      <c r="N35" s="2">
+        <v>0</v>
+      </c>
+      <c r="O35" s="2">
+        <v>0</v>
+      </c>
+      <c r="P35" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>0</v>
+      </c>
+      <c r="R35" s="2">
+        <v>0</v>
+      </c>
+      <c r="S35" s="2">
+        <v>0</v>
+      </c>
+      <c r="T35" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U35" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
+      <c r="A36" s="3">
         <v>-999</v>
-      </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="U35" s="2"/>
-    </row>
-    <row r="36" spans="1:21">
-      <c r="A36" s="4" t="s">
-        <v>0</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="U36" s="2"/>
+    </row>
+    <row r="37" spans="1:21">
+      <c r="A37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="U37" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2041,18 +2100,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2188,6 +2247,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0524FC3A-FFBB-4947-8673-B2AD9D6D8986}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03A630C0-0A26-4E8C-8075-3A67A467C74C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2199,14 +2266,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0524FC3A-FFBB-4947-8673-B2AD9D6D8986}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>